<commit_message>
first round Carnifex raid sim
</commit_message>
<xml_diff>
--- a/batch stuff/result.xlsx
+++ b/batch stuff/result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="8265" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="8265" firstSheet="1" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,12 @@
     <sheet name="Sheet11" sheetId="11" r:id="rId11"/>
     <sheet name="Sheet12" sheetId="12" r:id="rId12"/>
     <sheet name="Sheet13" sheetId="13" r:id="rId13"/>
+    <sheet name="Sheet14" sheetId="14" r:id="rId14"/>
+    <sheet name="Sheet15" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="NS_Allegiance_Brawl" localSheetId="9">Sheet10!$A$1:$C$62</definedName>
+    <definedName name="NS_Allegiance_Brawl_Enf_all" localSheetId="14">Sheet15!$A$1:$C$53</definedName>
     <definedName name="NS_Allegiance_Brawl_enfeed" localSheetId="10">Sheet11!$A$1:$C$49</definedName>
     <definedName name="NS_Allegiance_Brawl_Protect" localSheetId="11">Sheet12!$A$1:$C$49</definedName>
     <definedName name="NS_War_Def" localSheetId="4">Sheet5!$A$1:$D$51</definedName>
@@ -35,6 +38,9 @@
     <definedName name="NS_war_skyfort_IB" localSheetId="6">Sheet7!$A$1:$C$27</definedName>
     <definedName name="NS_war_skyfort_IB2" localSheetId="7">Sheet8!$A$1:$C$27</definedName>
     <definedName name="WH_Allegiance_Brawl" localSheetId="8">Sheet9!$A$1:$C$152</definedName>
+    <definedName name="WH_Allegiance_Brawl_Enf_all" localSheetId="13">Sheet14!$A$1:$C$25</definedName>
+    <definedName name="WH_Allegiance_Brawl_Enf_all2" localSheetId="13">Sheet14!$A$26:$C$33</definedName>
+    <definedName name="WH_Allegiance_Brawl_Enf_all3" localSheetId="13">Sheet14!$A$34:$C$51</definedName>
     <definedName name="WH_War_Def" localSheetId="5">Sheet6!$A$1:$D$51</definedName>
     <definedName name="WH_war_skyfort" localSheetId="2">Sheet3!$A$1:$C$51</definedName>
   </definedNames>
@@ -58,7 +64,16 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="NS_Allegiance_Brawl_enfeed" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="2" name="NS_Allegiance_Brawl_Enf_all" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\NS_Allegiance_Brawl_Enf_all.txt" tab="0" delimiter=":">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="NS_Allegiance_Brawl_enfeed" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\NS_Allegiance_Brawl_enfeed.txt" tab="0" delimiter=":">
       <textFields count="3">
         <textField/>
@@ -67,7 +82,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="NS_Allegiance_Brawl_Protect" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="4" name="NS_Allegiance_Brawl_Protect" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\NS_Allegiance_Brawl_Protect.txt" tab="0" delimiter=":">
       <textFields count="3">
         <textField/>
@@ -76,7 +91,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="NS_War_Def" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="5" name="NS_War_Def" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\NS_War_Def.txt" tab="0" delimiter=":">
       <textFields count="3">
         <textField/>
@@ -85,7 +100,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="NS_war_skyfort" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="6" name="NS_war_skyfort" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\NS_war_skyfort.txt" tab="0" delimiter=":">
       <textFields count="3">
         <textField/>
@@ -94,7 +109,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="NS_war_skyfort_IB" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="7" name="NS_war_skyfort_IB" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\NS_war_skyfort_IB.txt" tab="0" delimiter=":">
       <textFields count="3">
         <textField/>
@@ -103,7 +118,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="NS_war_skyfort_IB2" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="8" name="NS_war_skyfort_IB2" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\NS_war_skyfort_IB2.txt" tab="0" delimiter=":">
       <textFields count="3">
         <textField/>
@@ -112,7 +127,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="WH_Allegiance_Brawl" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="9" name="WH_Allegiance_Brawl" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\WH_Allegiance_Brawl.txt" tab="0" delimiter=":">
       <textFields count="3">
         <textField/>
@@ -121,7 +136,34 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="WH_War_Def" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="10" name="WH_Allegiance_Brawl_Enf_all" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\WH_Allegiance_Brawl_Enf_all.txt" tab="0" delimiter=":">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="11" name="WH_Allegiance_Brawl_Enf_all2" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\WH_Allegiance_Brawl_Enf_all2.txt" tab="0" delimiter=":">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="12" name="WH_Allegiance_Brawl_Enf_all3" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\WH_Allegiance_Brawl_Enf_all3.txt" tab="0" delimiter=":">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="13" name="WH_War_Def" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\WH_War_Def.txt" tab="0" delimiter=":">
       <textFields count="3">
         <textField/>
@@ -130,7 +172,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="WH_war_skyfort" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="14" name="WH_war_skyfort" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\jkim802\Documents\tu_opt\WH_war_skyfort.txt" tab="0" delimiter=":">
       <textFields count="3">
         <textField/>
@@ -143,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1615" uniqueCount="1059">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="1154">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -3320,6 +3362,291 @@
   </si>
   <si>
     <t>THE MASTRODAMUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Demi Constrictor, Arch Nova Alpha, Abhorrent Recluse, Inferno Demon, Baughe, Tazerecca, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lord Silus, Dreamhaunter, Shock Disruptor, Primus Ultima, Shock Disruptor, Sacred Sanctuary, Serrated Grater, Coldheart, Judgment Nova</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nexor, Dreamhaunter, Arch Nova Alpha, Xillanail, Tazerious, Jilted Baughe, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Arch Nova Alpha, Auger Ream, Inferno Demon, Bane of Truth, Tazerecca, Aggeroth Chaos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Demi Constrictor, Arch Nova Alpha, Abhorrent Recluse, Auger Ream, Jilted Baughe, Tazerecca, Bane of Truth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nexor, Demi Constrictor, Dreamhaunter, Xillanail, Inferno Demon, Baughe, Gorrus Rav, Steadfast Assailant</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lord Silus, Dreamhaunter, Shock Disruptor #2, Judgment Nova #2, Crude Surgeon, Inferno Demon, Guillotine Grinder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Demi Constrictor, Arch Nova Alpha, Inferno Demon, Jilted Baughe, Jilted Baughe-2, Bane of Truth, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Krellus, Xanadu Ultra, Dreamhaunter, Arch Nova Alpha, Jet, Abhorrent Recluse, Bane of Truth, Xillanail, Jilted Baughe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Arch Nova Alpha, Auger Ream, Jet, Bane of Truth, Jilted Baughe, Tazerecca, Trench Hurler</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Malort, Dreamhaunter, Ravenous Terrorsaur, Croc Oppressor #3, Aggeroth Chaos, Veiled Defiler</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tabitha, Octane's Bulwark, Sacred Sanctuary, Dreamhaunter, Hephatat Stoic, Jet, Bane of Truth, Auger Ream</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Demi Constrictor #2, Sacred Sanctuary, Arch Nova Alpha, Jilted Baughe, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Halcyon, Tundra MK3, Hoard Arsenal, Cruise Launcher, Galvanic Commando, Trigger Mark, Zealous Pursuer-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Arch Nova Alpha, Abhorrent Recluse, Jilted Baughe #2, Decorated Marshall, Bane of Truth, Lurker Behemoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Stoneheart, Sacred Sanctuary, Dreamhaunter, Xanadu Ultra, Demi Constrictor, Arch Nova Alpha, Bane of Truth, Steadfast Assailant</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Bolt Crag, Flash Deity, Sacred Sanctuary, Smite Forger, Coldheart, Zodiac Harbinger, Honorable Samurai</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lord Silus, Shock Disruptor, Dreamhaunter, Jet, Inferno Demon, Revolt Ranger, Bane of Truth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Arch Nova Alpha, Bane of Truth, Wilter Conscript, Xillanail, Honorable Samurai, Bolt Crag</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Dreamhaunter, Sacred Sanctuary, The Adversary, Arch Nova Alpha, Abhorrent Recluse, Inferno Demon, Jilted Baughe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Coldheart, Grand Templar, Arch Nova Alpha, Sacred Sanctuary, Blink Providence, Smite Forger, Zodiac Harbinger, Longshot Deadeye, Dreamreaper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Bane of Truth, Noble Defiance, Jilted Baughe, Baughe #2, Tazerecca, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kylen, Sacred Sanctuary, Demi Constrictor #2, Arch Nova Alpha, Jilted Baughe, Tazerecca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Dreamhaunter, Coldheart, Sacred Sanctuary, Smite Forger, Zodiac Harbinger #2, Noble Defiance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alaric, Halerift, Animus Geist, Dreamreaper, Jilted Baughe, Zodiac Harbinger #2, Dreamweaver</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Smite Forger #2, Zodiac Harbinger, Honorable Samurai, Zodiac Harbinger, Dreamreaper, Zodiac Harbinger</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Demi Constrictor, Arch Nova Alpha, Sacred Sanctuary, Abhorrent Recluse, Inferno Demon, Bane of Truth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kylen, Demi Constrictor, Dreamhaunter, Xanadu Ultra, Sacred Sanctuary, Arch Nova Alpha, Xillanail, Tazerecca, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Halcyon, Steel Ram, Octane's Bastion, Coldheart, Sculpted Aegis, Hephatat Stoic, Bane of Truth, Decorated Marshall, Steadfast Assailant</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Gehenna Cursed, Erebus City Sector, Ezamit Tranq, Scorched Hellwing #2, Erebus City Sector, Abhorrent Recluse</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nexor, Dreamhaunter, Arch Nova Alpha, Sacred Sanctuary, Abhorrent Recluse, Xillanail, Tazerecca, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cyrus, Infantry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Arch Nova Alpha, Abhorrent Recluse, Jilted Baughe, Tazerecca, Auger Bore, Noble Defiance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Demi Constrictor, Arch Nova Alpha, Auger Ream, Jilted Baughe, Tazerecca, Decorated Marshall, Bane of Truth-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Demi Constrictor, Sacred Sanctuary, Arch Nova Alpha, Ayrkrane Syn, Tazerious, Jilted Baughe, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Dreamhaunter, Coldheart, Sacred Sanctuary, Arch Nova Alpha, Smite Forger, Ayrkrane Syn, Noble Defiance, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Demi Constrictor, Serak United, Arch Nova Elite, Baughe #2, Sacred Sanctuary, Portal Noctil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nexor, Demi Constrictor, Sacred Sanctuary, Arch Nova Alpha, Honorable Samurai, Jilted Baughe, Bane of Truth, Tazerecca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Bolt Crag, Sacred Sanctuary, Smite Forger #2, Blink Providence, Divine Equalizer, Heroic Knight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Halcyon, Octane's Bastion, Hephatat Stoic, Jet, Guardian Gamut, Auger Ream, Bane of Truth, Dune Runner, Dreamreaper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Bolt Crag, Sacred Sanctuary, Bolt Crag, Flash Deity, Smite Forger, Deft Reclaimer, Dreamreaper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Demi Constrictor, Xanadu Ultra, Sacred Sanctuary, Arch Nova Alpha, The Adversary, Jilted Baughe, Tazerecca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Halcyon, Sculpted Aegis, Octane's Bastion, Cruise Launcher, Guardian Gamut, Hephatat Stoic, Auger Ream, Coldheart, Indestructible Troop</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Demi Constrictor, Arch Nova Alpha, Revolt Ranger, Bane of Truth, Baughe #2, Tazerecca, Dreamreaper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Dreamhaunter, Xanadu Ultra, Sacred Sanctuary, Demi Constrictor, Ezamit Tranq, Arch Nova Alpha, Tazerious, Auger Ream</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Demi Constrictor, Sacred Sanctuary, Arch Nova Alpha, Judgment Nova, Inferno Demon, Jilted Baughe, Bane of Truth</t>
+  </si>
+  <si>
+    <t>CLE4NSWEEPKID</t>
+  </si>
+  <si>
+    <t>Tylerurby</t>
+  </si>
+  <si>
+    <t>ajwiles13</t>
+  </si>
+  <si>
+    <t>johnoe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Stoneheart, Dreamhaunter, Sacred Sanctuary, Aggeroth Chaos, Arch Nova Alpha, Honorable Samurai, Tazerecca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Typhon Vex, Dreamhaunter, Obsidian, Stoneheart, Sacred Sanctuary, Portal Noctil, Tazerious</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Typhon Vex, Dreamhaunter, Obsidian, Stoneheart, Neo Dredge, Portal Noctil, Tazerecca</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Obsidian, Dreamhaunter, Stoneheart, Sacred Sanctuary #2, Ezamit Tranq, Arch Nova Alpha, Tazerious</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Daedalus, Obsidian, Dreamhaunter, Arch Nova Alpha, Tazerious, Jilted Baughe #2, Auger Ream</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Razor Pinion, Dirge, Rox Exterminator, Erebus City Sector, Scorched Hellwing, Flourish Turbine, Machina Awoken</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Typhon Vex, Dreamhaunter, Obsidian, Stoneheart, Sacred Sanctuary, Deserted Baughe, Portal Noctil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Typhon Vex, Dreamhaunter, Obsidian, Stoneheart, Sacred Sanctuary #2, Ezamit Tranq, Arch Nova Alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lord Silus, Shock Disruptor, Stoneheart, Sacred Sanctuary, Dreamhaunter, Erebus City Sector, Arch Nova Alpha, Oreworks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Razor Pinion, Tempest Citadel, Gehenna Cursed, Erebus City Sector, Scorched Hellwing, Dreamhaunter, Razor Pinion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nexor, Dreamhaunter, Stoneheart, Obsidian, Arch Nova Alpha, Jilted Baughe, Tazerecca, Ayrkrane Syn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tabitha, Octane's Bulwark, Obsidian, Dreamhaunter, Sacred Sanctuary, Bane of Truth, Auger Ream</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Obsidian, Arch Nova Alpha, Bane of Truth, Jilted Baughe, Tazerecca, Aggeroth Chaos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kylen, Obsidian, Dreamhaunter, Stoneheart, Sacred Sanctuary, Xillanail, Portal Noctil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tabitha, Octane's Bulwark, Auger Ream, Jet, Bane of Truth, Dune Runner, Decorated Marshall, Elite Squadron</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Stoneheart, Obsidian, Arch Nova Alpha, Auger Ream, Tazerecca, Aggeroth Chaos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kylen, Dreamhaunter, Stoneheart, Sacred Sanctuary, Demi Constrictor #2, Arch Nova Alpha, Xillanail, Sculpted Aegis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Bolt Crag, Coldheart, Sacred Sanctuary, Blink Providence, Grand Templar, Response Fleet, Dawn's Virtue, Honorable Samurai, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Arch Nova Alpha, Dune Runner, Jilted Baughe, Bane of Truth, Tazerecca, Lurker Behemoth</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nexor, Obsidian, Dreamhaunter, Stoneheart, Sacred Sanctuary #2, Abhorrent Recluse, Xanadu Ultra, Arch Nova Alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Typhon Vex, Dreamhaunter, Stoneheart, Sacred Sanctuary, Shock Disruptor, Judgment Nova #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Krellus, Obsidian, Dreamhaunter, Stoneheart, Serak United, Jilted Baughe, Honorable Samurai, Portal Noctil</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Stoneheart, Obsidian, Dreamhaunter, Sacred Sanctuary, Ayrkrane Syn, Honorable Samurai</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Kylen, Dreamhaunter, Demi Constrictor, Xillanail, Wilter Conscript, Tazerious, Jilted Baughe, Lurker Behemoth, Demi Constrictor, Coldheart</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Stoneheart, Obsidian, Sacred Sanctuary, Bolt Crag, Smite Forger, Samurai, Auger Ream</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, The Adversary, Obsidian, Sacred Sanctuary, Abhorrent Recluse, Arch Nova Alpha, Xanadu Ultra, Xillanail, Noble Defiance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Razor Pinion, Tempest Citadel, Gehenna Cursed, Erebus City Sector, Scorched Hellwing, Dreamhaunter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Constantine, Obsidian, Bolt Crag, Sacred Sanctuary, Erebus Outpost, Grand Templar, Bolt Crag, Lucifire</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Typhon Vex, Dreamhaunter, Stoneheart, Aggeroth Chaos, Tazerecca, Auger Bore</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Typhon Vex, Trench Hurler, Dreamhaunter, Obsidian, Stoneheart, Sacred Sanctuary, Tazerious, Judgment Nova</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Ayrkrane Syn, Abhorrent Recluse, Ezamit Tranq, Arch Nova Alpha, Jilted Baughe, Tazerious, Auger Ream, Noble Defiance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Gehenna Cursed, Erebus City Sector, Croc Oppressor, Jilted Baughe, Ardenmass, Erebus City Sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Obsidian, Arch Nova Alpha, Oreworks, Jilted Baughe-5, Tazerecca, Croc Oppressor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nexor, Xillanail, Arch Nova Alpha, Inferno Demon, Baughe, Tazerecca, Jet, Aggeroth Enraged</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Dreamhaunter, Stoneheart, Sacred Sanctuary, Obsidian, Abhorrent Recluse, Arch Nova Alpha, Tazerecca, Aggeroth Chaos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Typhon Vex, Dreamhaunter, Obsidian, Stoneheart, Sacred Sanctuary, Tazerious, Aggeroth Chaos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Daedalus, Obsidian, Dune Runner, Dreamhaunter, Arch Nova Alpha, Abhorrent Recluse #2, Jilted Baughe, Tazerious, Auger Ream</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Halcyon, Dreamhaunter, Obsidian, Stoneheart, Sacred Sanctuary, Bane of Truth, Guardian Gamut, Hephatat Stoic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Arch Nova Alpha, Oreworks, Erebus City Sector, Oreworks, Ayrkrane Syn, Bolt Crag</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Halcyon, Dreamhaunter, Stoneheart, Obsidian, Aggeroth Chaos, Tazerecca, Incog Niaq</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arkadios, Dreamhaunter, Gehenna Cursed, Erebus City Sector, Scorched Hellwing #2, Gehenna Cursed, Erebus City Sector, Machina Awoken</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Obsidian, Arch Nova Alpha, Revolt Ranger, Tazerious, Elite Squadron, Auger Ream</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tabitha, Dreamhaunter, Octane's Bulwark, Obsidian, Stoneheart, Sacred Sanctuary, Abhorrent Recluse, Auger Ream</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Barracus, Dreamhaunter, Obsidian, Arch Nova Alpha, Deserted Baughe, Tazerious, Auger Ream, Aggeroth Enraged</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lord Silus, Primus Ultima, Shock Disruptor #2, Dreamhaunter, Coldheart, Sacred Sanctuary, Judgment Nova, Serrated Grater, Crushing Anvil, Inferno Demon</t>
   </si>
 </sst>
 </file>
@@ -3595,13 +3922,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color rgb="FFCCCCCC"/>
         </left>
@@ -3611,6 +3931,13 @@
         <top style="medium">
           <color rgb="FFCCCCCC"/>
         </top>
+        <bottom style="medium">
+          <color rgb="FFCCCCCC"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color rgb="FFCCCCCC"/>
         </bottom>
@@ -3630,35 +3957,51 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="WH_war_skyfort" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="WH_war_skyfort" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_Allegiance_Brawl_Protect" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_Allegiance_Brawl_Protect" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="WH_Allegiance_Brawl_Enf_all3" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="WH_Allegiance_Brawl_Enf_all2" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="WH_Allegiance_Brawl_Enf_all" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_Allegiance_Brawl_Enf_all" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_war_skyfort" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_war_skyfort" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_War_Def" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_War_Def" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="WH_War_Def" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="WH_War_Def" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_war_skyfort_IB" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_war_skyfort_IB" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_war_skyfort_IB2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_war_skyfort_IB2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="WH_Allegiance_Brawl" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="WH_Allegiance_Brawl" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3666,11 +4009,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_Allegiance_Brawl_enfeed" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NS_Allegiance_Brawl_enfeed" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B340" totalsRowShown="0" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B340" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:B340"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Name" dataDxfId="1"/>
@@ -6185,7 +6528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D444"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B340"/>
     </sheetView>
   </sheetViews>
@@ -8689,6 +9032,1141 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1">
+        <v>78.638099999999994</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2">
+        <v>46.107599999999998</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3">
+        <v>37.093000000000004</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4">
+        <v>36.247599999999998</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5">
+        <v>30.7089</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B6">
+        <v>28.8386</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B7">
+        <v>27.7486</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8">
+        <v>25.6873</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B9">
+        <v>25.398900000000001</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10">
+        <v>24.6919</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11">
+        <v>24.2059</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B12">
+        <v>23.174299999999999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B13">
+        <v>23.0608</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B14">
+        <v>22.878599999999999</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B15">
+        <v>22.355399999999999</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B16">
+        <v>21.895399999999999</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17">
+        <v>21.4511</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18">
+        <v>21.4057</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B19">
+        <v>20.6738</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20">
+        <v>19.061399999999999</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21">
+        <v>18.716799999999999</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22">
+        <v>18.214600000000001</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B23">
+        <v>18.075399999999998</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B24">
+        <v>16.189699999999998</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B25">
+        <v>15.297599999999999</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B26">
+        <v>14.0632</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27">
+        <v>14.0573</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B28">
+        <v>14.0395</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B29">
+        <v>13.6632</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B30">
+        <v>13.3378</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31">
+        <v>12.981400000000001</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32">
+        <v>12.8527</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B33">
+        <v>12.6578</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B34">
+        <v>12.0854</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35">
+        <v>11.5768</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B36">
+        <v>9.2651400000000006</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B37">
+        <v>8.0070300000000003</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38">
+        <v>7.8483799999999997</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B39">
+        <v>6.2551399999999999</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B40">
+        <v>6.2137799999999999</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B41">
+        <v>6.0975700000000002</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B42">
+        <v>5.8391900000000003</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B43">
+        <v>5.7373000000000003</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B44">
+        <v>5.3754099999999996</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B45">
+        <v>2.7235100000000001</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1"/>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:C62">
+    <sortCondition descending="1" ref="B1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3">
+        <v>78.290999999999997</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B4">
+        <v>76.345500000000001</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>69.771000000000001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>64.695499999999996</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <v>48.779200000000003</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>48.133299999999998</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9">
+        <v>46.652500000000003</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <v>45.892000000000003</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
+        <v>43.822200000000002</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>42.810400000000001</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>42.3157</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>41.190399999999997</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>40.945900000000002</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16">
+        <v>39.980400000000003</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>38.411799999999999</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>37.787799999999997</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19">
+        <v>36.282400000000003</v>
+      </c>
+      <c r="C19" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B20">
+        <v>35.400599999999997</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>33.450000000000003</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>32.835900000000002</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23">
+        <v>32.436100000000003</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>29.268000000000001</v>
+      </c>
+      <c r="C24" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>29.124700000000001</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>28.986699999999999</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27">
+        <v>28.9496</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28">
+        <v>28.8871</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>28.345099999999999</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30">
+        <v>27.923100000000002</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>27.132000000000001</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>27.018999999999998</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>26.785699999999999</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>26.058199999999999</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35">
+        <v>25.560400000000001</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>25.406500000000001</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37">
+        <v>23.546900000000001</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <v>23.412700000000001</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>22.805299999999999</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40">
+        <v>21.688600000000001</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B41">
+        <v>17.406700000000001</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>16.441400000000002</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43">
+        <v>16.4251</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44">
+        <v>16.279800000000002</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45">
+        <v>15.749599999999999</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>13.0129</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47">
+        <v>12.1998</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48">
+        <v>11.410600000000001</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>5.61137</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50">
+        <v>3.7625500000000001</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1"/>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A3:C52">
+    <sortCondition descending="1" ref="B3"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>